<commit_message>
Initial output working. Need to delay MAC inputs by 2 clock cycles for second set of inputs.
</commit_message>
<xml_diff>
--- a/scheduling.xlsx
+++ b/scheduling.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="75">
   <si>
     <t>Cycle No.</t>
   </si>
@@ -235,6 +235,12 @@
   </si>
   <si>
     <t>Cycle</t>
+  </si>
+  <si>
+    <t>11(used to be a12)</t>
+  </si>
+  <si>
+    <t>Original</t>
   </si>
 </sst>
 </file>
@@ -454,7 +460,203 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="42">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1362,12 +1564,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="9"/>
   </cols>
   <sheetData>
@@ -1841,11 +2044,11 @@
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12">
-        <v>11</v>
+      <c r="A12" t="s">
+        <v>73</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>22</v>
@@ -1857,7 +2060,7 @@
         <v>22</v>
       </c>
       <c r="F12" s="10">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G12" s="10">
         <v>1010</v>
@@ -1872,7 +2075,7 @@
         <v>11</v>
       </c>
       <c r="K12" s="10">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="L12" s="10">
         <v>1010</v>
@@ -1889,7 +2092,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>23</v>
@@ -1901,7 +2104,7 @@
         <v>23</v>
       </c>
       <c r="F13" s="10">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="G13" s="10">
         <v>1011</v>
@@ -1916,7 +2119,7 @@
         <v>12</v>
       </c>
       <c r="K13" s="10">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="L13" s="10">
         <v>1011</v>
@@ -2200,46 +2403,46 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:I19 J2:J8 J11:J19">
-    <cfRule type="cellIs" dxfId="13" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="30" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="29" operator="equal">
       <formula>"a11"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="28" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="27" operator="equal">
       <formula>"a21"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="25">
+    <cfRule type="expression" dxfId="37" priority="25">
       <formula>OR(B2="a31", B2=10)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="24">
+    <cfRule type="expression" dxfId="36" priority="24">
       <formula>OR(B2="a12", B2=11)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="22">
+    <cfRule type="expression" dxfId="35" priority="22">
       <formula>OR(B2="a22", B2=100)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="21">
+    <cfRule type="expression" dxfId="34" priority="21">
       <formula>OR(B2="a32",B2=101)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="20">
+    <cfRule type="expression" dxfId="33" priority="20">
       <formula>OR(B2="a13", B2=110)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="19">
+    <cfRule type="expression" dxfId="32" priority="19">
       <formula>OR(B2="a23", B2=111)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="18">
+    <cfRule type="expression" dxfId="31" priority="18">
       <formula>OR(B2="a33", B2=1000)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="17">
+    <cfRule type="expression" dxfId="30" priority="17">
       <formula>OR(B2="a14",B2=1001)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="16">
+    <cfRule type="expression" dxfId="29" priority="16">
       <formula>OR(B2="a24", B2=1010)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="15">
+    <cfRule type="expression" dxfId="28" priority="15">
       <formula>OR(B2="a34", B2=1011)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2249,12 +2452,886 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="E2" s="9"/>
+      <c r="G2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="M2" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="N2" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="O2" s="34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="10">
+        <v>0</v>
+      </c>
+      <c r="H3" s="10">
+        <v>0</v>
+      </c>
+      <c r="I3" s="10">
+        <v>0</v>
+      </c>
+      <c r="J3" s="10">
+        <v>0</v>
+      </c>
+      <c r="K3" s="36">
+        <v>1</v>
+      </c>
+      <c r="L3" s="10">
+        <v>0</v>
+      </c>
+      <c r="M3" s="10">
+        <v>0</v>
+      </c>
+      <c r="N3" s="10">
+        <v>0</v>
+      </c>
+      <c r="O3" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="10">
+        <v>0</v>
+      </c>
+      <c r="H4" s="10">
+        <v>0</v>
+      </c>
+      <c r="I4" s="10">
+        <v>1</v>
+      </c>
+      <c r="J4" s="10">
+        <v>1</v>
+      </c>
+      <c r="K4" s="35">
+        <v>2</v>
+      </c>
+      <c r="L4" s="10">
+        <v>0</v>
+      </c>
+      <c r="M4" s="10">
+        <v>0</v>
+      </c>
+      <c r="N4" s="10">
+        <v>1</v>
+      </c>
+      <c r="O4" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="10">
+        <v>0</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0</v>
+      </c>
+      <c r="I5" s="10">
+        <v>10</v>
+      </c>
+      <c r="J5" s="10">
+        <v>10</v>
+      </c>
+      <c r="K5" s="35">
+        <v>3</v>
+      </c>
+      <c r="L5" s="10">
+        <v>0</v>
+      </c>
+      <c r="M5" s="10">
+        <v>0</v>
+      </c>
+      <c r="N5" s="10">
+        <v>10</v>
+      </c>
+      <c r="O5" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0</v>
+      </c>
+      <c r="H6" s="10">
+        <v>11</v>
+      </c>
+      <c r="I6" s="10">
+        <v>11</v>
+      </c>
+      <c r="J6" s="10">
+        <v>11</v>
+      </c>
+      <c r="K6" s="35">
+        <v>4</v>
+      </c>
+      <c r="L6" s="10">
+        <v>0</v>
+      </c>
+      <c r="M6" s="10">
+        <v>11</v>
+      </c>
+      <c r="N6" s="10">
+        <v>11</v>
+      </c>
+      <c r="O6" s="10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="10">
+        <v>1</v>
+      </c>
+      <c r="H7" s="10">
+        <v>100</v>
+      </c>
+      <c r="I7" s="10">
+        <v>100</v>
+      </c>
+      <c r="J7" s="10">
+        <v>100</v>
+      </c>
+      <c r="K7" s="35">
+        <v>5</v>
+      </c>
+      <c r="L7" s="10">
+        <v>1</v>
+      </c>
+      <c r="M7" s="10">
+        <v>100</v>
+      </c>
+      <c r="N7" s="10">
+        <v>100</v>
+      </c>
+      <c r="O7" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="10">
+        <v>10</v>
+      </c>
+      <c r="H8" s="10">
+        <v>101</v>
+      </c>
+      <c r="I8" s="10">
+        <v>101</v>
+      </c>
+      <c r="J8" s="10">
+        <v>101</v>
+      </c>
+      <c r="K8" s="35">
+        <v>6</v>
+      </c>
+      <c r="L8" s="10">
+        <v>10</v>
+      </c>
+      <c r="M8" s="10">
+        <v>101</v>
+      </c>
+      <c r="N8" s="10">
+        <v>101</v>
+      </c>
+      <c r="O8" s="10">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0</v>
+      </c>
+      <c r="H9" s="10">
+        <v>110</v>
+      </c>
+      <c r="I9" s="10">
+        <v>110</v>
+      </c>
+      <c r="J9" s="10">
+        <v>110</v>
+      </c>
+      <c r="K9" s="35">
+        <v>7</v>
+      </c>
+      <c r="L9" s="10">
+        <v>0</v>
+      </c>
+      <c r="M9" s="10">
+        <v>110</v>
+      </c>
+      <c r="N9" s="10">
+        <v>110</v>
+      </c>
+      <c r="O9" s="10">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="10">
+        <v>111</v>
+      </c>
+      <c r="I10" s="10">
+        <v>111</v>
+      </c>
+      <c r="J10" s="10">
+        <v>111</v>
+      </c>
+      <c r="K10" s="35">
+        <v>8</v>
+      </c>
+      <c r="L10" s="10">
+        <v>1</v>
+      </c>
+      <c r="M10" s="10">
+        <v>111</v>
+      </c>
+      <c r="N10" s="10">
+        <v>111</v>
+      </c>
+      <c r="O10" s="10">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="10">
+        <v>10</v>
+      </c>
+      <c r="H11" s="10">
+        <v>1000</v>
+      </c>
+      <c r="I11" s="10">
+        <v>1000</v>
+      </c>
+      <c r="J11" s="10">
+        <v>1000</v>
+      </c>
+      <c r="K11" s="35">
+        <v>9</v>
+      </c>
+      <c r="L11" s="10">
+        <v>10</v>
+      </c>
+      <c r="M11" s="10">
+        <v>1000</v>
+      </c>
+      <c r="N11" s="10">
+        <v>1000</v>
+      </c>
+      <c r="O11" s="10">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0</v>
+      </c>
+      <c r="H12" s="10">
+        <v>1001</v>
+      </c>
+      <c r="I12" s="10">
+        <v>1001</v>
+      </c>
+      <c r="J12" s="10">
+        <v>1001</v>
+      </c>
+      <c r="K12" s="35">
+        <v>10</v>
+      </c>
+      <c r="L12" s="10">
+        <v>0</v>
+      </c>
+      <c r="M12" s="10">
+        <v>1001</v>
+      </c>
+      <c r="N12" s="10">
+        <v>1001</v>
+      </c>
+      <c r="O12" s="10">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="B13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="10">
+        <v>1</v>
+      </c>
+      <c r="H13" s="10">
+        <v>1010</v>
+      </c>
+      <c r="I13" s="10">
+        <v>1010</v>
+      </c>
+      <c r="J13" s="10">
+        <v>1010</v>
+      </c>
+      <c r="K13" s="35">
+        <v>11</v>
+      </c>
+      <c r="L13" s="10">
+        <v>1</v>
+      </c>
+      <c r="M13" s="10">
+        <v>1010</v>
+      </c>
+      <c r="N13" s="10">
+        <v>1010</v>
+      </c>
+      <c r="O13" s="10">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="10">
+        <v>110</v>
+      </c>
+      <c r="H14" s="10">
+        <v>1011</v>
+      </c>
+      <c r="I14" s="10">
+        <v>1011</v>
+      </c>
+      <c r="J14" s="10">
+        <v>1011</v>
+      </c>
+      <c r="K14" s="35">
+        <v>12</v>
+      </c>
+      <c r="L14" s="10">
+        <v>110</v>
+      </c>
+      <c r="M14" s="10">
+        <v>1011</v>
+      </c>
+      <c r="N14" s="10">
+        <v>1011</v>
+      </c>
+      <c r="O14" s="10">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="10">
+        <v>11</v>
+      </c>
+      <c r="H15" s="10">
+        <v>110</v>
+      </c>
+      <c r="I15" s="10">
+        <v>11</v>
+      </c>
+      <c r="J15" s="10">
+        <v>1001</v>
+      </c>
+      <c r="K15" s="35">
+        <v>13</v>
+      </c>
+      <c r="L15" s="10">
+        <v>11</v>
+      </c>
+      <c r="M15" s="10">
+        <v>110</v>
+      </c>
+      <c r="N15" s="10">
+        <v>11</v>
+      </c>
+      <c r="O15" s="10">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="10">
+        <v>100</v>
+      </c>
+      <c r="H16" s="10">
+        <v>111</v>
+      </c>
+      <c r="I16" s="10">
+        <v>100</v>
+      </c>
+      <c r="J16" s="10">
+        <v>1010</v>
+      </c>
+      <c r="K16" s="35">
+        <v>14</v>
+      </c>
+      <c r="L16" s="10">
+        <v>100</v>
+      </c>
+      <c r="M16" s="10">
+        <v>111</v>
+      </c>
+      <c r="N16" s="10">
+        <v>100</v>
+      </c>
+      <c r="O16" s="10">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15">
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="10">
+        <v>101</v>
+      </c>
+      <c r="H17" s="10">
+        <v>1000</v>
+      </c>
+      <c r="I17" s="10">
+        <v>101</v>
+      </c>
+      <c r="J17" s="10">
+        <v>1011</v>
+      </c>
+      <c r="K17" s="35">
+        <v>15</v>
+      </c>
+      <c r="L17" s="10">
+        <v>101</v>
+      </c>
+      <c r="M17" s="10">
+        <v>1000</v>
+      </c>
+      <c r="N17" s="10">
+        <v>101</v>
+      </c>
+      <c r="O17" s="10">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15">
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="10">
+        <v>110</v>
+      </c>
+      <c r="H18" s="10">
+        <v>1001</v>
+      </c>
+      <c r="I18" s="10">
+        <v>0</v>
+      </c>
+      <c r="J18" s="10">
+        <v>0</v>
+      </c>
+      <c r="K18" s="35">
+        <v>16</v>
+      </c>
+      <c r="L18" s="10">
+        <v>110</v>
+      </c>
+      <c r="M18" s="10">
+        <v>1001</v>
+      </c>
+      <c r="N18" s="10">
+        <v>0</v>
+      </c>
+      <c r="O18" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15">
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="10">
+        <v>111</v>
+      </c>
+      <c r="H19" s="10">
+        <v>1010</v>
+      </c>
+      <c r="I19" s="10">
+        <v>0</v>
+      </c>
+      <c r="J19" s="10">
+        <v>0</v>
+      </c>
+      <c r="K19" s="35">
+        <v>17</v>
+      </c>
+      <c r="L19" s="10">
+        <v>111</v>
+      </c>
+      <c r="M19" s="10">
+        <v>1010</v>
+      </c>
+      <c r="N19" s="10">
+        <v>0</v>
+      </c>
+      <c r="O19" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15">
+      <c r="B20">
+        <v>18</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="10">
+        <v>1000</v>
+      </c>
+      <c r="H20" s="10">
+        <v>1011</v>
+      </c>
+      <c r="I20" s="10">
+        <v>0</v>
+      </c>
+      <c r="J20" s="10">
+        <v>0</v>
+      </c>
+      <c r="K20" s="35">
+        <v>18</v>
+      </c>
+      <c r="L20" s="10">
+        <v>1000</v>
+      </c>
+      <c r="M20" s="10">
+        <v>1011</v>
+      </c>
+      <c r="N20" s="10">
+        <v>0</v>
+      </c>
+      <c r="O20" s="10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C3:J20 K3:K9 K12:K20">
+    <cfRule type="expression" dxfId="14" priority="1">
+      <formula>OR(C3="a34", C3=1011)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="2">
+      <formula>OR(C3="a24", C3=1010)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="3">
+      <formula>OR(C3="a14",C3=1001)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="4">
+      <formula>OR(C3="a33", C3=1000)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="5">
+      <formula>OR(C3="a23", C3=111)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="6">
+      <formula>OR(C3="a13", C3=110)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="7">
+      <formula>OR(C3="a32",C3=101)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="8">
+      <formula>OR(C3="a22", C3=100)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="9">
+      <formula>OR(C3="a12", C3=11)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="10">
+      <formula>OR(C3="a31", C3=10)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="11" operator="equal">
+      <formula>"a21"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="12" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="13" operator="equal">
+      <formula>"a11"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="14" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>